<commit_message>
Incorporacion de Logica para Join con Efectores solapa SIF-SIGEHOS
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/EfectoresObjetivos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/EfectoresObjetivos.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personales\Sistemas\Agustin\Reportes BI\2021\Facturación\Version 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="87">
   <si>
     <t>sif</t>
   </si>
@@ -255,12 +255,42 @@
   </si>
   <si>
     <t>Talleres protegidos</t>
+  </si>
+  <si>
+    <t>Talleres Protegidos</t>
+  </si>
+  <si>
+    <t>Curie</t>
+  </si>
+  <si>
+    <t>Ferrer</t>
+  </si>
+  <si>
+    <t>Ramos Mejia</t>
+  </si>
+  <si>
+    <t>Santa Lucia</t>
+  </si>
+  <si>
+    <t>Sarda</t>
+  </si>
+  <si>
+    <t>Tornu</t>
+  </si>
+  <si>
+    <t>Quinquela Martin</t>
+  </si>
+  <si>
+    <t>Tobar Garcia</t>
+  </si>
+  <si>
+    <t>EfectorSigehos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,15 +383,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:C38" totalsRowShown="0">
-  <autoFilter ref="A1:C38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:D38" totalsRowShown="0">
+  <autoFilter ref="A1:D38"/>
   <sortState ref="A2:C38">
     <sortCondition ref="A1:A38"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="3" name="ID"/>
     <tableColumn id="1" name="sif"/>
     <tableColumn id="2" name="EfectorObjetivos"/>
+    <tableColumn id="4" name="EfectorSigehos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -633,16 +664,17 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="57.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>73</v>
       </c>
@@ -652,8 +684,11 @@
       <c r="C1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -663,8 +698,11 @@
       <c r="C2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -674,8 +712,11 @@
       <c r="C3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -685,8 +726,11 @@
       <c r="C4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -696,8 +740,11 @@
       <c r="C5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -707,8 +754,11 @@
       <c r="C6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -718,8 +768,11 @@
       <c r="C7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -729,8 +782,11 @@
       <c r="C8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -740,8 +796,11 @@
       <c r="C9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -751,8 +810,11 @@
       <c r="C10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -762,8 +824,11 @@
       <c r="C11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -773,8 +838,11 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -784,8 +852,11 @@
       <c r="C13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -795,8 +866,11 @@
       <c r="C14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -806,8 +880,11 @@
       <c r="C15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -817,8 +894,11 @@
       <c r="C16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -828,8 +908,11 @@
       <c r="C17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19</v>
       </c>
@@ -839,8 +922,11 @@
       <c r="C18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20</v>
       </c>
@@ -850,8 +936,11 @@
       <c r="C19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21</v>
       </c>
@@ -861,8 +950,11 @@
       <c r="C20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>22</v>
       </c>
@@ -872,8 +964,11 @@
       <c r="C21" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>23</v>
       </c>
@@ -883,8 +978,11 @@
       <c r="C22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>24</v>
       </c>
@@ -894,8 +992,11 @@
       <c r="C23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
@@ -905,8 +1006,11 @@
       <c r="C24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
@@ -916,8 +1020,11 @@
       <c r="C25" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>424</v>
       </c>
@@ -927,8 +1034,11 @@
       <c r="C26" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>425</v>
       </c>
@@ -938,8 +1048,11 @@
       <c r="C27" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>702</v>
       </c>
@@ -949,8 +1062,11 @@
       <c r="C28" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>704</v>
       </c>
@@ -960,8 +1076,11 @@
       <c r="C29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>938</v>
       </c>
@@ -971,8 +1090,11 @@
       <c r="C30" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1466</v>
       </c>
@@ -982,8 +1104,11 @@
       <c r="C31" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1607</v>
       </c>
@@ -992,6 +1117,9 @@
       </c>
       <c r="C32" t="s">
         <v>76</v>
+      </c>
+      <c r="D32" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1004,6 +1132,9 @@
       <c r="C33" t="s">
         <v>64</v>
       </c>
+      <c r="D33" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -1015,6 +1146,9 @@
       <c r="C34" t="s">
         <v>67</v>
       </c>
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -1026,6 +1160,9 @@
       <c r="C35" t="s">
         <v>44</v>
       </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -1037,6 +1174,9 @@
       <c r="C36" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
@@ -1048,6 +1188,9 @@
       <c r="C37" t="s">
         <v>38</v>
       </c>
+      <c r="D37" t="s">
+        <v>38</v>
+      </c>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1058,6 +1201,9 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambio de la funcion ReadSigehosData para interpretar exports de Sigehos
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/EfectoresObjetivos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/EfectoresObjetivos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="129">
   <si>
     <t>sif</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Talleres Protegidos</t>
   </si>
   <si>
-    <t>Curie</t>
-  </si>
-  <si>
     <t>Ferrer</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
     <t>EfectorSigehos</t>
   </si>
   <si>
-    <t>ALVAREZ</t>
-  </si>
-  <si>
     <t>ALVEAR</t>
   </si>
   <si>
@@ -305,9 +299,6 @@
     <t>CARRILLO</t>
   </si>
   <si>
-    <t>CURIE</t>
-  </si>
-  <si>
     <t>DE QUEMADOS</t>
   </si>
   <si>
@@ -332,18 +323,12 @@
     <t>GUTIERREZ</t>
   </si>
   <si>
-    <t>Maria Ferrer</t>
-  </si>
-  <si>
     <t>Jose Dueñas</t>
   </si>
   <si>
     <t>LAGLEYZE</t>
   </si>
   <si>
-    <t>Marie Curie</t>
-  </si>
-  <si>
     <t>MOYANO</t>
   </si>
   <si>
@@ -417,6 +402,15 @@
   </si>
   <si>
     <t>MostrarGrafico</t>
+  </si>
+  <si>
+    <t>HOSP..MUNICIPAL.DE.ONCOLOGIA.M..CURIE</t>
+  </si>
+  <si>
+    <t>HOSP..GENERAL.DE.AGUDOS.DR.T..ALVAREZ</t>
+  </si>
+  <si>
+    <t>HOSP..DE.REHABILITACION.RESPIRATORIA.M..FERRER</t>
   </si>
 </sst>
 </file>
@@ -508,8 +502,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E87" totalsRowShown="0">
-  <autoFilter ref="A1:E87"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:E83" totalsRowShown="0">
+  <autoFilter ref="A1:E83"/>
   <sortState ref="A2:E60">
     <sortCondition ref="E2"/>
   </sortState>
@@ -787,17 +781,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="57.5703125" customWidth="1"/>
     <col min="3" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -811,10 +805,10 @@
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -831,24 +825,24 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>1644</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -865,24 +859,24 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1644</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -899,24 +893,24 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>13</v>
+        <v>3118</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -933,24 +927,24 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3118</v>
+        <v>424</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -967,24 +961,24 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>424</v>
+        <v>1855</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,1282 +995,1214 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1855</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>21</v>
+        <v>704</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6</v>
+        <v>704</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>704</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>704</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9</v>
+        <v>2678</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>9</v>
+        <v>2678</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2678</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="1">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2678</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="1">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>19</v>
+        <v>702</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>19</v>
+        <v>704</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>702</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>704</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>12</v>
+        <v>425</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>9</v>
+        <v>425</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D36">
         <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>425</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>425</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D42">
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D43">
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D44">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>2</v>
+        <v>1466</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
       <c r="E46" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>2</v>
+        <v>1466</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>6</v>
+        <v>1466</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="E48" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>6</v>
+        <v>1466</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1466</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D50">
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>1466</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1466</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>1466</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D53">
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D54">
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
       <c r="E56" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>14</v>
+        <v>2334</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D57">
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>14</v>
+        <v>2334</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D58">
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>2334</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2334</v>
+        <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>117</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C64" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C65" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C66" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>3</v>
+        <v>1607</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="D67">
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>24</v>
+        <v>1607</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C68" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>24</v>
+        <v>938</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D69">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>24</v>
+        <v>938</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C70" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D70">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>1607</v>
+        <v>938</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C71" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>1607</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D72">
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>938</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>938</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>938</v>
+        <v>3140</v>
       </c>
       <c r="B75" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C75" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>20</v>
+        <v>3140</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C76" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>20</v>
+        <v>3140</v>
       </c>
       <c r="B77" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C77" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D78">
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3140</v>
+        <v>15</v>
       </c>
       <c r="B79" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>3140</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C80" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>3140</v>
+        <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C81" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D81">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D82">
         <v>2</v>
       </c>
       <c r="E82" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D83">
         <v>2</v>
       </c>
       <c r="E83" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>16</v>
-      </c>
-      <c r="B84" t="s">
-        <v>20</v>
-      </c>
-      <c r="C84" t="s">
-        <v>57</v>
-      </c>
-      <c r="D84">
-        <v>1</v>
-      </c>
-      <c r="E84" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>16</v>
-      </c>
-      <c r="B85" t="s">
-        <v>20</v>
-      </c>
-      <c r="C85" t="s">
-        <v>57</v>
-      </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>22</v>
-      </c>
-      <c r="B86" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86" t="s">
-        <v>46</v>
-      </c>
-      <c r="D86">
-        <v>2</v>
-      </c>
-      <c r="E86" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>22</v>
-      </c>
-      <c r="B87" t="s">
-        <v>9</v>
-      </c>
-      <c r="C87" t="s">
-        <v>46</v>
-      </c>
-      <c r="D87">
-        <v>2</v>
-      </c>
-      <c r="E87" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>